<commit_message>
Made the modal add new study sets
</commit_message>
<xml_diff>
--- a/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/All flashcards.xlsx
+++ b/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/All flashcards.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -125,13 +125,53 @@
   </si>
   <si>
     <t>this is a very llong long long long long long long longlongong long long long long long long longlong long long long long long long long longlong long long long long long long long longlong long long long long long long long longlong long long long long long long long longlong long long long long long long long longlong long long long long long long long longlong long long long long long long long longlong question</t>
+  </si>
+  <si>
+    <t>2023-10-08 02:25:54 9_4_1179775</t>
+  </si>
+  <si>
+    <t>test test</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>2023-10-08 02:34:14 9_4_3835979</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="31">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="164" formatCode="General"/>
@@ -196,7 +236,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23:C26"/>
@@ -488,6 +528,28 @@
       </c>
       <c r="C26" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="1048569" ht="12.8"/>

</xml_diff>

<commit_message>
Added new functionalities with requirements + some style
</commit_message>
<xml_diff>
--- a/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/All flashcards.xlsx
+++ b/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/All flashcards.xlsx
@@ -182,7 +182,37 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="48">
+  <numFmts count="78">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>

</xml_diff>

<commit_message>
added linq and optional parameter
</commit_message>
<xml_diff>
--- a/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/All flashcards.xlsx
+++ b/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/All flashcards.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -176,13 +176,24 @@
   </si>
   <si>
     <t>aaa</t>
+  </si>
+  <si>
+    <t>2023-10-17 13:42:35 6 question_6_2</t>
+  </si>
+  <si>
+    <t>6 question</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="78">
+  <numFmts count="80">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
@@ -322,7 +333,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23:C26"/>
@@ -735,6 +746,17 @@
       </c>
       <c r="C37" s="0" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="1048569" ht="12.8"/>

</xml_diff>

<commit_message>
new controller is added
</commit_message>
<xml_diff>
--- a/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/All flashcards.xlsx
+++ b/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/All flashcards.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -185,13 +185,24 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>2023-10-22 21:36:58 7 question_7_8530875</t>
+  </si>
+  <si>
+    <t>7 question</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="80">
+  <numFmts count="82">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
@@ -333,7 +344,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23:C26"/>
@@ -757,6 +768,17 @@
       </c>
       <c r="C38" s="0" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="1048569" ht="12.8"/>

</xml_diff>